<commit_message>
Dataset with years [2]
</commit_message>
<xml_diff>
--- a/migforecasting/cities19-21/1/d10.xlsx
+++ b/migforecasting/cities19-21/1/d10.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\cities19-21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\cities19-21\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -5390,8 +5390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BI79" sqref="BI79"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BL2" sqref="BL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5617,7 +5617,194 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:65" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:65" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2019</v>
+      </c>
+      <c r="C4">
+        <v>2019</v>
+      </c>
+      <c r="D4">
+        <v>2019</v>
+      </c>
+      <c r="E4">
+        <v>2019</v>
+      </c>
+      <c r="F4">
+        <v>2019</v>
+      </c>
+      <c r="G4">
+        <v>2019</v>
+      </c>
+      <c r="H4">
+        <v>2019</v>
+      </c>
+      <c r="I4">
+        <v>2019</v>
+      </c>
+      <c r="J4">
+        <v>2019</v>
+      </c>
+      <c r="K4">
+        <v>2019</v>
+      </c>
+      <c r="L4">
+        <v>2019</v>
+      </c>
+      <c r="M4">
+        <v>2019</v>
+      </c>
+      <c r="N4">
+        <v>2019</v>
+      </c>
+      <c r="O4">
+        <v>2019</v>
+      </c>
+      <c r="P4">
+        <v>2019</v>
+      </c>
+      <c r="Q4">
+        <v>2019</v>
+      </c>
+      <c r="R4">
+        <v>2019</v>
+      </c>
+      <c r="S4">
+        <v>2019</v>
+      </c>
+      <c r="T4">
+        <v>2019</v>
+      </c>
+      <c r="U4">
+        <v>2019</v>
+      </c>
+      <c r="V4">
+        <v>2019</v>
+      </c>
+      <c r="W4">
+        <v>2020</v>
+      </c>
+      <c r="X4">
+        <v>2020</v>
+      </c>
+      <c r="Y4">
+        <v>2020</v>
+      </c>
+      <c r="Z4">
+        <v>2020</v>
+      </c>
+      <c r="AA4">
+        <v>2020</v>
+      </c>
+      <c r="AB4">
+        <v>2020</v>
+      </c>
+      <c r="AC4">
+        <v>2020</v>
+      </c>
+      <c r="AD4">
+        <v>2020</v>
+      </c>
+      <c r="AE4">
+        <v>2020</v>
+      </c>
+      <c r="AF4">
+        <v>2020</v>
+      </c>
+      <c r="AG4">
+        <v>2020</v>
+      </c>
+      <c r="AH4">
+        <v>2020</v>
+      </c>
+      <c r="AI4">
+        <v>2020</v>
+      </c>
+      <c r="AJ4">
+        <v>2020</v>
+      </c>
+      <c r="AK4">
+        <v>2020</v>
+      </c>
+      <c r="AL4">
+        <v>2020</v>
+      </c>
+      <c r="AM4">
+        <v>2020</v>
+      </c>
+      <c r="AN4">
+        <v>2020</v>
+      </c>
+      <c r="AO4">
+        <v>2020</v>
+      </c>
+      <c r="AP4">
+        <v>2020</v>
+      </c>
+      <c r="AQ4">
+        <v>2020</v>
+      </c>
+      <c r="AR4">
+        <v>2021</v>
+      </c>
+      <c r="AS4">
+        <v>2021</v>
+      </c>
+      <c r="AT4">
+        <v>2021</v>
+      </c>
+      <c r="AU4">
+        <v>2021</v>
+      </c>
+      <c r="AV4">
+        <v>2021</v>
+      </c>
+      <c r="AW4">
+        <v>2021</v>
+      </c>
+      <c r="AX4">
+        <v>2021</v>
+      </c>
+      <c r="AY4">
+        <v>2021</v>
+      </c>
+      <c r="AZ4">
+        <v>2021</v>
+      </c>
+      <c r="BA4">
+        <v>2021</v>
+      </c>
+      <c r="BB4">
+        <v>2021</v>
+      </c>
+      <c r="BC4">
+        <v>2021</v>
+      </c>
+      <c r="BD4">
+        <v>2021</v>
+      </c>
+      <c r="BE4">
+        <v>2021</v>
+      </c>
+      <c r="BF4">
+        <v>2021</v>
+      </c>
+      <c r="BG4">
+        <v>2021</v>
+      </c>
+      <c r="BH4">
+        <v>2021</v>
+      </c>
+      <c r="BI4">
+        <v>2021</v>
+      </c>
+      <c r="BJ4">
+        <v>2021</v>
+      </c>
+      <c r="BK4">
+        <v>2021</v>
+      </c>
+    </row>
     <row r="5" spans="1:65" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>

</xml_diff>